<commit_message>
Final changes are published
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deves\Desktop\Origin\Certificate Generation Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6107736-7E89-44C5-88E4-C9DD80626DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC22054-DA00-49F4-8689-B4B41D516034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Contact Info</t>
-  </si>
-  <si>
-    <t>Devesh Rawat</t>
   </si>
   <si>
     <t>Astha</t>
@@ -357,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -379,7 +376,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>7078140054</v>
@@ -387,25 +384,9 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>8394870189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>7078140054</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
         <v>7078140054</v>
       </c>
     </row>

</xml_diff>